<commit_message>
Split tests and create logic for Write results to file
</commit_message>
<xml_diff>
--- a/core/src/test/resources/result.xlsx
+++ b/core/src/test/resources/result.xlsx
@@ -20,13 +20,13 @@
     <t>Номер кузова</t>
   </si>
   <si>
-    <t>KMHBT51DBBU022069</t>
+    <t>KMHBT51DBBU022001</t>
   </si>
   <si>
-    <t>KMHSU81XDDU112496</t>
+    <t>KMHSU81XDDU112002</t>
   </si>
   <si>
-    <t>KMHEC41BBCA350931</t>
+    <t>KMHEC41BBCA350003</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Create links to found VINs in result file
</commit_message>
<xml_diff>
--- a/core/src/test/resources/result.xlsx
+++ b/core/src/test/resources/result.xlsx
@@ -43,12 +43,32 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="52"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkGrid">
+        <bgColor indexed="52"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkGrid">
+        <bgColor indexed="17"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -63,8 +83,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -83,17 +105,17 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="1">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Play around with colors. Find the most suitable
</commit_message>
<xml_diff>
--- a/core/src/test/resources/result.xlsx
+++ b/core/src/test/resources/result.xlsx
@@ -43,7 +43,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -70,6 +70,16 @@
         <bgColor indexed="17"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill>
+        <bgColor rgb="FF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkGrid">
+        <bgColor rgb="FF0000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -83,10 +93,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -105,17 +118,17 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="1">
+      <c r="A2" t="s" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="1">
+      <c r="A3" t="s" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="1">
+      <c r="A4" t="s" s="5">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Set foreground color instead of background. Test in Windows 2013
</commit_message>
<xml_diff>
--- a/core/src/test/resources/result.xlsx
+++ b/core/src/test/resources/result.xlsx
@@ -43,7 +43,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -52,32 +52,22 @@
     </fill>
     <fill>
       <patternFill>
-        <bgColor indexed="52"/>
+        <fgColor rgb="FF0000"/>
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="darkGrid">
-        <bgColor indexed="52"/>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill>
-        <bgColor indexed="17"/>
+        <fgColor rgb="33FF33"/>
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="darkGrid">
-        <bgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill>
-        <bgColor rgb="FF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="darkGrid">
-        <bgColor rgb="FF0000"/>
+      <patternFill patternType="solid">
+        <fgColor rgb="33FF33"/>
       </patternFill>
     </fill>
   </fills>
@@ -93,13 +83,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -110,7 +97,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="17"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -118,17 +105,17 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="4">
+      <c r="A3" t="s" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="5">
+      <c r="A4" t="s" s="1">
         <v>4</v>
       </c>
     </row>

</xml_diff>